<commit_message>
update excel linked charts to local files... fk rules fk visio
</commit_message>
<xml_diff>
--- a/data/ablation.xlsx
+++ b/data/ablation.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView windowWidth="26880" windowHeight="12975"/>
   </bookViews>
@@ -1436,19 +1436,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>17.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>15.23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,19 +1569,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>17.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>14.83</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.91</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1921,19 +1921,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>21.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>18.65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.59</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.94</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,19 +2054,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>14.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>12.39</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.62</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.87</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2399,19 +2399,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>17.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>14.71</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.34</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.82</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2532,19 +2532,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>11.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>9.45</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.28</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.63</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7593,11 +7593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7942,28 +7942,32 @@
         <v>14</v>
       </c>
       <c r="G9">
-        <v>15.23</v>
+        <v>17.86</v>
       </c>
       <c r="H9">
-        <v>14.83</v>
-      </c>
+        <v>17.25</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="K9" t="s">
         <v>14</v>
       </c>
       <c r="L9">
-        <v>18.65</v>
+        <v>21.59</v>
       </c>
       <c r="M9">
-        <v>12.39</v>
-      </c>
+        <v>14.62</v>
+      </c>
+      <c r="N9"/>
+      <c r="O9"/>
       <c r="P9" t="s">
         <v>14</v>
       </c>
       <c r="Q9">
-        <v>14.71</v>
+        <v>17.34</v>
       </c>
       <c r="R9">
-        <v>9.45</v>
+        <v>11.28</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7980,28 +7984,32 @@
         <v>15</v>
       </c>
       <c r="G10">
-        <v>17.86</v>
+        <v>18.42</v>
       </c>
       <c r="H10">
-        <v>17.25</v>
-      </c>
+        <v>17.91</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" t="s">
         <v>15</v>
       </c>
       <c r="L10">
-        <v>21.59</v>
+        <v>22.17</v>
       </c>
       <c r="M10">
-        <v>14.62</v>
-      </c>
+        <v>15.13</v>
+      </c>
+      <c r="N10"/>
+      <c r="O10"/>
       <c r="P10" t="s">
         <v>15</v>
       </c>
       <c r="Q10">
-        <v>17.34</v>
+        <v>17.96</v>
       </c>
       <c r="R10">
-        <v>11.28</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -8018,28 +8026,32 @@
         <v>16</v>
       </c>
       <c r="G11">
-        <v>18.42</v>
+        <v>17.15</v>
       </c>
       <c r="H11">
-        <v>17.91</v>
-      </c>
+        <v>16.58</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" t="s">
         <v>16</v>
       </c>
       <c r="L11">
-        <v>22.17</v>
+        <v>20.94</v>
       </c>
       <c r="M11">
-        <v>15.13</v>
-      </c>
+        <v>13.87</v>
+      </c>
+      <c r="N11"/>
+      <c r="O11"/>
       <c r="P11" t="s">
         <v>16</v>
       </c>
       <c r="Q11">
-        <v>17.96</v>
+        <v>16.82</v>
       </c>
       <c r="R11">
-        <v>11.75</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -8056,28 +8068,32 @@
         <v>17</v>
       </c>
       <c r="G12">
-        <v>17.15</v>
+        <v>16.37</v>
       </c>
       <c r="H12">
-        <v>16.58</v>
-      </c>
+        <v>15.74</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12"/>
       <c r="K12" t="s">
         <v>17</v>
       </c>
       <c r="L12">
-        <v>20.94</v>
+        <v>19.78</v>
       </c>
       <c r="M12">
-        <v>13.87</v>
-      </c>
+        <v>13.15</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
       <c r="P12" t="s">
         <v>17</v>
       </c>
       <c r="Q12">
-        <v>16.82</v>
+        <v>15.69</v>
       </c>
       <c r="R12">
-        <v>10.63</v>
+        <v>10.12</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -8094,28 +8110,32 @@
         <v>18</v>
       </c>
       <c r="G13">
-        <v>16.37</v>
+        <v>15.23</v>
       </c>
       <c r="H13">
-        <v>15.74</v>
-      </c>
+        <v>14.83</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13"/>
       <c r="K13" t="s">
         <v>18</v>
       </c>
       <c r="L13">
-        <v>19.78</v>
+        <v>18.65</v>
       </c>
       <c r="M13">
-        <v>13.15</v>
-      </c>
+        <v>12.39</v>
+      </c>
+      <c r="N13"/>
+      <c r="O13"/>
       <c r="P13" t="s">
         <v>18</v>
       </c>
       <c r="Q13">
-        <v>15.69</v>
+        <v>14.71</v>
       </c>
       <c r="R13">
-        <v>10.12</v>
+        <v>9.45</v>
       </c>
     </row>
     <row r="33" spans="12:14">
@@ -8191,7 +8211,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8208,7 +8228,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>